<commit_message>
Atualização automática de TRAMANDAI.xlsx
</commit_message>
<xml_diff>
--- a/TRAMANDAI.xlsx
+++ b/TRAMANDAI.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{997BDBF3-B665-4200-9C05-2B90611404C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F73926A-05DA-43FF-ABE0-50D2F081423A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Paineis DARQ" sheetId="10" r:id="rId1"/>
+    <sheet name="Paineis DARQ" sheetId="11" r:id="rId1"/>
     <sheet name="DESFAZIMENTOS" sheetId="1" r:id="rId2"/>
     <sheet name="MATERIAIS-FORNECIDOS" sheetId="2" r:id="rId3"/>
     <sheet name="DATA-LIMITE-REQUISICOES" sheetId="3" r:id="rId4"/>
@@ -23,13 +23,14 @@
     <sheet name="TCA" sheetId="7" r:id="rId8"/>
     <sheet name="Recolhimento x Eliminacao" sheetId="8" r:id="rId9"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="9" r:id="rId10"/>
+    <sheet name="DGC" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="437">
   <si>
     <t>COMARCA</t>
   </si>
@@ -1326,6 +1327,24 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>TEMÁTICA</t>
+  </si>
+  <si>
+    <t>PROBLEMA</t>
+  </si>
+  <si>
+    <t>MOT-VIG</t>
+  </si>
+  <si>
+    <t>Validou posto que não existe na comarca</t>
+  </si>
+  <si>
+    <t>MOT-Limpeza</t>
+  </si>
+  <si>
+    <t>Demora nos Atestes MOT</t>
   </si>
 </sst>
 </file>
@@ -1336,7 +1355,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot; &quot;mmmm&quot; / &quot;yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1389,6 +1408,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1403,7 +1435,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1444,6 +1476,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB7E1CD"/>
         <bgColor rgb="FFB7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
@@ -1529,9 +1567,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1623,12 +1661,16 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{F4B8CC2A-099B-4A4D-93F2-9034644F4F8D}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{E862D167-9430-4449-9CDA-4EDCAA19FB82}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1658,10 +1700,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87045F9E-F1BC-45CD-AEFD-E84A3712BDED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{867DEB6B-852E-4AE5-9387-2B51166DFEC9}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1699,7 +1741,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E194D8A-CBB5-4A0D-B1DE-43148E4B9F56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15791B64-72D3-4BCB-AC6E-C3358BF89F2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1762,7 +1804,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEA1E079-E681-4C01-A9AB-5C85F89F552C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{864B8A79-4221-41CF-8FE0-0E9FA6B3AD51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1781,7 +1823,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7FD527E-3E52-7C16-7087-5A445E00B8B9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFFD77BA-6E37-F155-6727-BEEEE390C9E1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1830,7 +1872,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E34678B6-B661-39B0-FCCC-A3C794802BBA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69572D29-AE02-AEEF-0473-CE14CAC7883E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1849,7 +1891,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B742BC63-B969-43A8-B0A1-3F444BEF54F8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E239D6F-FA1A-0A14-97E7-BCC12BA2D065}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1880,7 +1922,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09061E1A-6515-93AB-D28F-D65D11DD1FDC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{332E7A34-82E8-DA55-5B29-DB58CB055DF1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1911,7 +1953,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{947E83AD-DA0A-7FEA-FFA5-DEB26AE922A6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C831EE48-8AA3-489C-2DC4-AE4B3FD14D19}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1954,7 +1996,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6817459-F335-406F-9159-5D32DDC3F045}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A3B6256-25CC-4CCC-BFE0-90267691D1FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1992,7 +2034,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C8A32E7-860A-411D-88E0-B7FA7AC5DFB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6617CC2F-AA56-420D-99FE-65A56C4FBA11}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2035,7 +2077,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CE5D2E1-B883-4F32-8A39-4FB0BF278EA3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBE7F591-A141-4414-94C6-4D4FA016ED74}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2348,7 +2390,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D81713D9-3F5D-4D8D-880C-DD602A828951}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F45FFA3-D31F-4FC8-AB4E-CBB5B0066679}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2360,98 +2402,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="40"/>
-    <col min="6" max="6" width="2" style="40" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="40" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="40"/>
+    <col min="1" max="5" width="12.5703125" style="42"/>
+    <col min="6" max="6" width="2" style="42" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="42" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="42"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="39"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="39"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="39"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="39"/>
+      <c r="F4" s="41"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="39"/>
+      <c r="F5" s="41"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="39"/>
+      <c r="F10" s="41"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="39"/>
+      <c r="F11" s="41"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="39"/>
+      <c r="F12" s="41"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="39"/>
+      <c r="F13" s="41"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="39"/>
+      <c r="F14" s="41"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="39"/>
+      <c r="F15" s="41"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="39"/>
+      <c r="F16" s="41"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="39"/>
+      <c r="F17" s="41"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="39"/>
+      <c r="F18" s="41"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="39"/>
+      <c r="F19" s="41"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="39"/>
+      <c r="F20" s="41"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="39"/>
+      <c r="F21" s="41"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="39"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="39"/>
+      <c r="F23" s="41"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="39"/>
+      <c r="F24" s="41"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="39"/>
+      <c r="F25" s="41"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="39"/>
+      <c r="F26" s="41"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="39"/>
+      <c r="F27" s="41"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="39"/>
+      <c r="F28" s="41"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="39"/>
+      <c r="F29" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -2500,6 +2542,57 @@
       </c>
       <c r="C2" s="36">
         <v>4.0999867742362124E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="88.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>431</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>433</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>435</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>